<commit_message>
backfilled the totals column!
</commit_message>
<xml_diff>
--- a/df2.xlsx
+++ b/df2.xlsx
@@ -498,7 +498,9 @@
       <c r="G2" t="n">
         <v>24</v>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -528,7 +530,9 @@
       <c r="G3" t="n">
         <v>158</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -558,7 +562,9 @@
       <c r="G4" t="n">
         <v>29</v>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -588,7 +594,9 @@
       <c r="G5" t="n">
         <v>103</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -650,7 +658,9 @@
       <c r="G7" t="n">
         <v>34</v>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -680,7 +690,9 @@
       <c r="G8" t="n">
         <v>144</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -710,7 +722,9 @@
       <c r="G9" t="n">
         <v>28</v>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -740,7 +754,9 @@
       <c r="G10" t="n">
         <v>15</v>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -802,7 +818,9 @@
       <c r="G12" t="n">
         <v>86</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -832,7 +850,9 @@
       <c r="G13" t="n">
         <v>198</v>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -862,7 +882,9 @@
       <c r="G14" t="n">
         <v>18</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -892,7 +914,9 @@
       <c r="G15" t="n">
         <v>25</v>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -954,7 +978,9 @@
       <c r="G17" t="n">
         <v>41</v>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -984,7 +1010,9 @@
       <c r="G18" t="n">
         <v>152</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1014,7 +1042,9 @@
       <c r="G19" t="n">
         <v>23</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1076,7 +1106,9 @@
       <c r="G21" t="n">
         <v>115</v>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>260</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1106,7 +1138,9 @@
       <c r="G22" t="n">
         <v>93</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>260</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1136,7 +1170,9 @@
       <c r="G23" t="n">
         <v>39</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>260</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1166,7 +1202,9 @@
       <c r="G24" t="n">
         <v>13</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>260</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1228,7 +1266,9 @@
       <c r="G26" t="n">
         <v>80</v>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1258,7 +1298,9 @@
       <c r="G27" t="n">
         <v>135</v>
       </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="H27" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1288,7 +1330,9 @@
       <c r="G28" t="n">
         <v>24</v>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1318,7 +1362,9 @@
       <c r="G29" t="n">
         <v>23</v>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1380,7 +1426,9 @@
       <c r="G31" t="n">
         <v>15</v>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1410,7 +1458,9 @@
       <c r="G32" t="n">
         <v>150</v>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1440,7 +1490,9 @@
       <c r="G33" t="n">
         <v>20</v>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1470,7 +1522,9 @@
       <c r="G34" t="n">
         <v>0</v>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1532,7 +1586,9 @@
       <c r="G36" t="n">
         <v>56</v>
       </c>
-      <c r="H36" t="inlineStr"/>
+      <c r="H36" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1562,7 +1618,9 @@
       <c r="G37" t="n">
         <v>163</v>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1592,7 +1650,9 @@
       <c r="G38" t="n">
         <v>19</v>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1622,7 +1682,9 @@
       <c r="G39" t="n">
         <v>5</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1684,7 +1746,9 @@
       <c r="G41" t="n">
         <v>71</v>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1714,7 +1778,9 @@
       <c r="G42" t="n">
         <v>158</v>
       </c>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1744,7 +1810,9 @@
       <c r="G43" t="n">
         <v>13</v>
       </c>
-      <c r="H43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1774,7 +1842,9 @@
       <c r="G44" t="n">
         <v>19</v>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">

</xml_diff>